<commit_message>
Add an Option Window
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82324D89-7103-40D1-83DA-06514515B68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96915357-95F2-49CD-B31A-095AB0F2D57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="2175" windowWidth="16815" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
@@ -491,9 +491,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -645,7 +647,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
@@ -653,7 +655,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
@@ -677,7 +679,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
@@ -702,6 +704,142 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add the suggestion feature
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -1,33 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96915357-95F2-49CD-B31A-095AB0F2D57F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19470" windowHeight="6150"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
     <sheet name="上部结构" sheetId="2" r:id="rId2"/>
     <sheet name="下部结构" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+  <si>
+    <t>序号</t>
+  </si>
   <si>
     <t>位置</t>
   </si>
@@ -59,18 +51,27 @@
     <t>左幅0#伸缩缝沉积物阻塞</t>
   </si>
   <si>
+    <t>855,858</t>
+  </si>
+  <si>
     <t>接缝处铺装碎边</t>
   </si>
   <si>
     <t>左幅0#伸缩缝接缝处铺装碎边</t>
   </si>
   <si>
+    <t>868</t>
+  </si>
+  <si>
     <t>右幅0#伸缩缝沉积物阻塞</t>
   </si>
   <si>
     <t>右幅1#伸缩缝沉积物阻塞</t>
   </si>
   <si>
+    <t>855,858,875</t>
+  </si>
+  <si>
     <t>栏杆</t>
   </si>
   <si>
@@ -89,6 +90,9 @@
     <t>左幅主梁</t>
   </si>
   <si>
+    <t>855</t>
+  </si>
+  <si>
     <t>右幅主梁</t>
   </si>
   <si>
@@ -116,9 +120,15 @@
     <t>左幅1#台台身露筋锈蚀</t>
   </si>
   <si>
+    <t>858</t>
+  </si>
+  <si>
     <t>右幅1#台台身露筋锈蚀</t>
   </si>
   <si>
+    <t>875</t>
+  </si>
+  <si>
     <t>支座</t>
   </si>
   <si>
@@ -126,69 +136,373 @@
   </si>
   <si>
     <t>右幅支座完好</t>
-  </si>
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>855,858</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>868</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>855,858,875</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>855</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>868</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>858</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>875</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -196,9 +510,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -212,17 +768,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -271,7 +871,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -306,7 +906,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -480,168 +1080,163 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -649,7 +1244,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -657,7 +1252,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -665,7 +1260,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -673,7 +1268,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -681,7 +1276,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -689,7 +1284,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -697,7 +1292,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -705,7 +1300,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -713,7 +1308,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -721,7 +1316,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -729,7 +1324,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -737,7 +1332,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -745,7 +1340,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -753,7 +1348,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -761,7 +1356,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -769,7 +1364,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -777,7 +1372,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -785,7 +1380,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -793,7 +1388,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -801,7 +1396,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -809,7 +1404,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -817,7 +1412,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -825,7 +1420,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -833,7 +1428,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -842,98 +1437,99 @@
       <c r="G31" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1501B7A2-AA81-40D9-9750-EC1FE7C158FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -941,7 +1537,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -949,7 +1545,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -957,7 +1553,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -965,7 +1561,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -973,7 +1569,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -982,190 +1578,191 @@
       <c r="G9" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29A3D48-2E34-4711-AE59-F4F03DE1DEC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="4" max="4" width="15.125" customWidth="1"/>
+    <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upgrade the table header name
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEE5011-99A4-4FB8-80A4-458925455BEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38E2A1B-6103-43CC-B340-4E501F8DF2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3825" windowWidth="28125" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="675" yWindow="3045" windowWidth="28125" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>序号</t>
   </si>
@@ -144,6 +144,10 @@
   </si>
   <si>
     <t>缺损描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>构件类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -831,7 +835,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -849,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>
@@ -968,7 +974,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -986,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
fix a bug in SaveExcel
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFEBC70-A3FB-43D8-A338-169DB672DE18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738DB2F9-B57E-49E1-B15A-5EBC49C40E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="48">
   <si>
     <t>序号</t>
   </si>
@@ -156,6 +156,26 @@
   </si>
   <si>
     <t>新增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位1数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位2数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用自定义单位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +194,14 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -198,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -210,6 +238,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -499,9 +530,10 @@
     <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +558,23 @@
       <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -550,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -576,7 +623,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -597,7 +644,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -623,7 +670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -646,7 +693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -654,7 +701,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -662,7 +709,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -670,7 +717,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -678,7 +725,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -686,7 +733,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -694,7 +741,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -702,7 +749,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -710,7 +757,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -718,7 +765,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -855,9 +902,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -865,9 +914,10 @@
     <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
+    <col min="9" max="9" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,8 +942,23 @@
       <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -916,7 +981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -940,7 +1005,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -948,7 +1013,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -956,7 +1021,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -964,7 +1029,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -972,7 +1037,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -980,7 +1045,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -996,9 +1061,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:M1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1006,9 +1073,10 @@
     <col min="4" max="4" width="15.125" customWidth="1"/>
     <col min="5" max="6" width="27.875" customWidth="1"/>
     <col min="7" max="7" width="25.25" customWidth="1"/>
+    <col min="9" max="9" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1033,8 +1101,23 @@
       <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1057,7 +1140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1081,7 +1164,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1107,7 +1190,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1130,7 +1213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1153,7 +1236,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
finish the feature IntactStructNoInsertSummaryTable
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VsProjects\AutoRegularInspection\AutoRegularInspection\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D9B087-C866-4114-81C5-1B66269D438D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5895" yWindow="3360" windowWidth="19515" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
     <sheet name="上部结构" sheetId="2" r:id="rId2"/>
     <sheet name="下部结构" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="135">
   <si>
     <t>序号</t>
   </si>
@@ -45,6 +39,9 @@
     <t>照片编号</t>
   </si>
   <si>
+    <t>自定义照片编号</t>
+  </si>
+  <si>
     <t>备注</t>
   </si>
   <si>
@@ -69,7 +66,7 @@
     <t>桥面铺装</t>
   </si>
   <si>
-    <t>完好</t>
+    <t>/</t>
   </si>
   <si>
     <t>桥面铺装完好</t>
@@ -97,349 +94,12 @@
   </si>
   <si>
     <t>2732</t>
-  </si>
-  <si>
-    <t>处</t>
-  </si>
-  <si>
-    <t>米</t>
-  </si>
-  <si>
-    <t>接缝处裂缝</t>
-  </si>
-  <si>
-    <t>0#台伸缩缝接缝处铺装裂缝，累计12条</t>
-  </si>
-  <si>
-    <t>0#台伸缩缝接缝处铺装裂缝</t>
-  </si>
-  <si>
-    <t>2737-1</t>
-  </si>
-  <si>
-    <t>条</t>
-  </si>
-  <si>
-    <t>3#台伸缩缝止水带多处破损，长度累计为2m</t>
-  </si>
-  <si>
-    <t>3#台伸缩缝止水带多处破损</t>
-  </si>
-  <si>
-    <t>2776</t>
-  </si>
-  <si>
-    <t>3#台伸缩缝接缝处铺装裂缝，累计7条</t>
-  </si>
-  <si>
-    <t>3#台伸缩缝接缝处铺装裂缝</t>
-  </si>
-  <si>
-    <t>2776-1</t>
-  </si>
-  <si>
-    <t>两侧型钢高差</t>
-  </si>
-  <si>
-    <t>0#台伸缩缝两侧型钢高差</t>
-  </si>
-  <si>
-    <t>2834</t>
-  </si>
-  <si>
-    <t>3#台伸缩缝两侧型钢高差</t>
-  </si>
-  <si>
-    <t>2833</t>
-  </si>
-  <si>
-    <t>栏杆</t>
-  </si>
-  <si>
-    <t>表层油漆剥落、锈蚀</t>
-  </si>
-  <si>
-    <t>全桥栏杆多处表层油漆剥落、锈蚀</t>
-  </si>
-  <si>
-    <t>2743,2744</t>
-  </si>
-  <si>
-    <t>构件类型</t>
-  </si>
-  <si>
-    <t>主梁</t>
-  </si>
-  <si>
-    <t>主梁梁底整体照</t>
-  </si>
-  <si>
-    <t>2804</t>
-  </si>
-  <si>
-    <t>水蚀</t>
-  </si>
-  <si>
-    <t>主梁翼板及腹板外侧大面积水蚀，面积约占主梁翼板总面积30%</t>
-  </si>
-  <si>
-    <t>主梁翼板及腹板外侧大面积水蚀</t>
-  </si>
-  <si>
-    <t>2807,2808</t>
-  </si>
-  <si>
-    <t>主梁3#台位置外侧腹板水蚀</t>
-  </si>
-  <si>
-    <t>2788,2789</t>
-  </si>
-  <si>
-    <t>表面裂缝</t>
-  </si>
-  <si>
-    <t>主梁横梁存在表面裂缝</t>
-  </si>
-  <si>
-    <t>主梁横梁表面裂缝</t>
-  </si>
-  <si>
-    <t>2835,2858</t>
-  </si>
-  <si>
-    <t>索塔</t>
-  </si>
-  <si>
-    <t>1#索塔上塔柱完好</t>
-  </si>
-  <si>
-    <t>2811-1</t>
-  </si>
-  <si>
-    <t>1#索塔下塔柱水蚀</t>
-  </si>
-  <si>
-    <t>2824</t>
-  </si>
-  <si>
-    <t>2#索塔上塔柱完好</t>
-  </si>
-  <si>
-    <t>2771</t>
-  </si>
-  <si>
-    <t>2#索塔下塔柱水蚀</t>
-  </si>
-  <si>
-    <t>2832</t>
-  </si>
-  <si>
-    <t>主缆</t>
-  </si>
-  <si>
-    <t>主缆外观完好</t>
-  </si>
-  <si>
-    <t>2811-1,2812</t>
-  </si>
-  <si>
-    <t>主缆锚固系统</t>
-  </si>
-  <si>
-    <t>2782</t>
-  </si>
-  <si>
-    <t>索夹</t>
-  </si>
-  <si>
-    <t>锈蚀</t>
-  </si>
-  <si>
-    <t>全桥索夹螺母轻微锈蚀，累计38处</t>
-  </si>
-  <si>
-    <t>全桥索夹螺母轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2752,2753</t>
-  </si>
-  <si>
-    <t>吊杆</t>
-  </si>
-  <si>
-    <t>ZDG-15吊杆锚杯轻微锈蚀，S=0.05×0.05m2</t>
-  </si>
-  <si>
-    <t>ZDG-15吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2772</t>
-  </si>
-  <si>
-    <t>平方米</t>
-  </si>
-  <si>
-    <t>ZDG-18吊杆锚杯轻微锈蚀，S=0.15×0.10m2</t>
-  </si>
-  <si>
-    <t>ZDG-18吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2774</t>
-  </si>
-  <si>
-    <t>ZDG-19吊杆锚杯轻微锈蚀，S=0.30×0.10m2</t>
-  </si>
-  <si>
-    <t>ZDG-19吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2775</t>
-  </si>
-  <si>
-    <t>YDG-5吊杆锚杯及密封筒轻微锈蚀，S=0.10×0.04m2</t>
-  </si>
-  <si>
-    <t>YDG-5吊杆锚杯及密封筒轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2818</t>
-  </si>
-  <si>
-    <t>YDG-13吊杆锚杯轻微锈蚀，S=0.05×0.05m2</t>
-  </si>
-  <si>
-    <t>YDG-13吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2768</t>
-  </si>
-  <si>
-    <t>YDG-15吊杆锚杯轻微锈蚀，S=0.08×0.03m2</t>
-  </si>
-  <si>
-    <t>YDG-15吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2773</t>
-  </si>
-  <si>
-    <t>YDG-16吊杆锚杯轻微锈蚀，S=0.10×0.10m2</t>
-  </si>
-  <si>
-    <t>YDG-16吊杆锚杯轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2765</t>
-  </si>
-  <si>
-    <t>全桥多处吊杆叉耳锈蚀</t>
-  </si>
-  <si>
-    <t>2814,2815</t>
-  </si>
-  <si>
-    <t>吊杆下锚头</t>
-  </si>
-  <si>
-    <t>吊杆下锚头完好</t>
-  </si>
-  <si>
-    <t>2799,2800</t>
-  </si>
-  <si>
-    <t>0#台</t>
-  </si>
-  <si>
-    <t>支座</t>
-  </si>
-  <si>
-    <t>钢垫板锈蚀</t>
-  </si>
-  <si>
-    <t>0-1#支座钢垫板锈蚀</t>
-  </si>
-  <si>
-    <t>2828</t>
-  </si>
-  <si>
-    <t>0-2#支座钢垫板锈蚀</t>
-  </si>
-  <si>
-    <t>2822</t>
-  </si>
-  <si>
-    <t>1#墩</t>
-  </si>
-  <si>
-    <t>1-1#支座钢垫板轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2853</t>
-  </si>
-  <si>
-    <t>1-2#支座钢垫板轻微锈蚀</t>
-  </si>
-  <si>
-    <t>2854</t>
-  </si>
-  <si>
-    <t>2#墩</t>
-  </si>
-  <si>
-    <t>2-1#支座钢垫板轻微锈蚀</t>
-  </si>
-  <si>
-    <t>15052</t>
-  </si>
-  <si>
-    <t>2-2#支座钢垫板轻微锈蚀</t>
-  </si>
-  <si>
-    <t>115252</t>
-  </si>
-  <si>
-    <t>3#台</t>
-  </si>
-  <si>
-    <t>3-1#支座钢垫板锈蚀</t>
-  </si>
-  <si>
-    <t>2796</t>
-  </si>
-  <si>
-    <t>3-2#支座钢垫板锈蚀</t>
-  </si>
-  <si>
-    <t>2795</t>
-  </si>
-  <si>
-    <t>桥台背墙</t>
-  </si>
-  <si>
-    <t>3#桥台背墙水蚀</t>
-  </si>
-  <si>
-    <t>2783,2785</t>
-  </si>
-  <si>
-    <t>自定义照片编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>照片编号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>备注</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
       <rPr>
         <sz val="11"/>
         <rFont val="宋体"/>
-        <family val="3"/>
         <charset val="134"/>
       </rPr>
       <t>附图</t>
@@ -448,49 +108,714 @@
       <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>1-1</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>处</t>
+  </si>
+  <si>
+    <t>米</t>
+  </si>
+  <si>
+    <t>接缝处裂缝</t>
+  </si>
+  <si>
+    <t>0#台伸缩缝接缝处铺装裂缝，累计12条</t>
+  </si>
+  <si>
+    <t>0#台伸缩缝接缝处铺装裂缝</t>
+  </si>
+  <si>
+    <t>2737-1</t>
+  </si>
+  <si>
+    <t>条</t>
+  </si>
+  <si>
+    <t>3#台伸缩缝止水带多处破损，长度累计为2m</t>
+  </si>
+  <si>
+    <t>3#台伸缩缝止水带多处破损</t>
+  </si>
+  <si>
+    <t>2776</t>
+  </si>
+  <si>
+    <t>3#台伸缩缝接缝处铺装裂缝，累计7条</t>
+  </si>
+  <si>
+    <t>3#台伸缩缝接缝处铺装裂缝</t>
+  </si>
+  <si>
+    <t>2776-1</t>
+  </si>
+  <si>
+    <t>两侧型钢高差</t>
+  </si>
+  <si>
+    <t>0#台伸缩缝两侧型钢高差</t>
+  </si>
+  <si>
+    <t>2834</t>
+  </si>
+  <si>
+    <t>3#台伸缩缝两侧型钢高差</t>
+  </si>
+  <si>
+    <t>2833</t>
+  </si>
+  <si>
+    <t>栏杆</t>
+  </si>
+  <si>
+    <t>表层油漆剥落、锈蚀</t>
+  </si>
+  <si>
+    <t>全桥栏杆多处表层油漆剥落、锈蚀</t>
+  </si>
+  <si>
+    <t>2743,2744</t>
+  </si>
+  <si>
+    <t>构件类型</t>
+  </si>
+  <si>
+    <t>主梁</t>
+  </si>
+  <si>
+    <t>主梁梁底整体照</t>
+  </si>
+  <si>
+    <t>2804</t>
+  </si>
+  <si>
+    <t>水蚀</t>
+  </si>
+  <si>
+    <t>主梁翼板及腹板外侧大面积水蚀，面积约占主梁翼板总面积30%</t>
+  </si>
+  <si>
+    <t>主梁翼板及腹板外侧大面积水蚀</t>
+  </si>
+  <si>
+    <t>2807,2808</t>
+  </si>
+  <si>
+    <t>主梁3#台位置外侧腹板水蚀</t>
+  </si>
+  <si>
+    <t>2788,2789</t>
+  </si>
+  <si>
+    <t>表面裂缝</t>
+  </si>
+  <si>
+    <t>主梁横梁存在表面裂缝</t>
+  </si>
+  <si>
+    <t>主梁横梁表面裂缝</t>
+  </si>
+  <si>
+    <t>2835,2858</t>
+  </si>
+  <si>
+    <t>索塔</t>
+  </si>
+  <si>
+    <t>1#索塔上塔柱完好</t>
+  </si>
+  <si>
+    <t>2811-1</t>
+  </si>
+  <si>
+    <t>1#索塔下塔柱水蚀</t>
+  </si>
+  <si>
+    <t>2824</t>
+  </si>
+  <si>
+    <t>2#索塔上塔柱完好</t>
+  </si>
+  <si>
+    <t>2771</t>
+  </si>
+  <si>
+    <t>2#索塔下塔柱水蚀</t>
+  </si>
+  <si>
+    <t>2832</t>
+  </si>
+  <si>
+    <t>主缆</t>
+  </si>
+  <si>
+    <t>主缆外观完好</t>
+  </si>
+  <si>
+    <t>2811-1,2812</t>
+  </si>
+  <si>
+    <t>主缆锚固系统</t>
+  </si>
+  <si>
+    <t>2782</t>
+  </si>
+  <si>
+    <t>索夹</t>
+  </si>
+  <si>
+    <t>锈蚀</t>
+  </si>
+  <si>
+    <t>全桥索夹螺母轻微锈蚀，累计38处</t>
+  </si>
+  <si>
+    <t>全桥索夹螺母轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2752,2753</t>
+  </si>
+  <si>
+    <t>吊杆</t>
+  </si>
+  <si>
+    <t>ZDG-15吊杆锚杯轻微锈蚀，S=0.05×0.05m2</t>
+  </si>
+  <si>
+    <t>ZDG-15吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2772</t>
+  </si>
+  <si>
+    <t>平方米</t>
+  </si>
+  <si>
+    <t>ZDG-18吊杆锚杯轻微锈蚀，S=0.15×0.10m2</t>
+  </si>
+  <si>
+    <t>ZDG-18吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2774</t>
+  </si>
+  <si>
+    <t>ZDG-19吊杆锚杯轻微锈蚀，S=0.30×0.10m2</t>
+  </si>
+  <si>
+    <t>ZDG-19吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2775</t>
+  </si>
+  <si>
+    <t>YDG-5吊杆锚杯及密封筒轻微锈蚀，S=0.10×0.04m2</t>
+  </si>
+  <si>
+    <t>YDG-5吊杆锚杯及密封筒轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2818</t>
+  </si>
+  <si>
+    <t>YDG-13吊杆锚杯轻微锈蚀，S=0.05×0.05m2</t>
+  </si>
+  <si>
+    <t>YDG-13吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2768</t>
+  </si>
+  <si>
+    <t>YDG-15吊杆锚杯轻微锈蚀，S=0.08×0.03m2</t>
+  </si>
+  <si>
+    <t>YDG-15吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2773</t>
+  </si>
+  <si>
+    <t>YDG-16吊杆锚杯轻微锈蚀，S=0.10×0.10m2</t>
+  </si>
+  <si>
+    <t>YDG-16吊杆锚杯轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2765</t>
+  </si>
+  <si>
+    <t>全桥多处吊杆叉耳锈蚀</t>
+  </si>
+  <si>
+    <t>2814,2815</t>
+  </si>
+  <si>
+    <t>吊杆下锚头</t>
+  </si>
+  <si>
+    <t>吊杆下锚头完好</t>
+  </si>
+  <si>
+    <t>2799,2800</t>
+  </si>
+  <si>
+    <t>0#台</t>
+  </si>
+  <si>
+    <t>支座</t>
+  </si>
+  <si>
+    <t>钢垫板锈蚀</t>
+  </si>
+  <si>
+    <t>0-1#支座钢垫板锈蚀</t>
+  </si>
+  <si>
+    <t>2828</t>
+  </si>
+  <si>
+    <t>0-2#支座钢垫板锈蚀</t>
+  </si>
+  <si>
+    <t>2822</t>
+  </si>
+  <si>
+    <t>1#墩</t>
+  </si>
+  <si>
+    <t>1-1#支座钢垫板轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2853</t>
+  </si>
+  <si>
+    <t>1-2#支座钢垫板轻微锈蚀</t>
+  </si>
+  <si>
+    <t>2854</t>
+  </si>
+  <si>
+    <t>2#墩</t>
+  </si>
+  <si>
+    <t>2-1#支座钢垫板轻微锈蚀</t>
+  </si>
+  <si>
+    <t>15052</t>
+  </si>
+  <si>
+    <t>2-2#支座钢垫板轻微锈蚀</t>
+  </si>
+  <si>
+    <t>115252</t>
+  </si>
+  <si>
+    <t>3#台</t>
+  </si>
+  <si>
+    <t>3-1#支座钢垫板锈蚀</t>
+  </si>
+  <si>
+    <t>2796</t>
+  </si>
+  <si>
+    <t>3-2#支座钢垫板锈蚀</t>
+  </si>
+  <si>
+    <t>2795</t>
+  </si>
+  <si>
+    <t>桥台背墙</t>
+  </si>
+  <si>
+    <t>3#桥台背墙水蚀</t>
+  </si>
+  <si>
+    <t>2783,2785</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -498,24 +823,311 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -564,7 +1176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -597,26 +1209,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -649,23 +1244,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,24 +1385,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -849,350 +1425,356 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>2</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>136</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K6">
         <v>7</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:I1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="13.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="22.1428571428571" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -1202,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1214,598 +1796,598 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
+        <v>63</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
+        <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
+        <v>72</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
+        <v>72</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K12">
         <v>38</v>
       </c>
       <c r="L12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M13">
-        <v>2.5000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M14">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M15">
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M16">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1813,37 +2395,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G17" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M17">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1851,37 +2433,37 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M18">
-        <v>2.3999999999999998E-3</v>
+        <v>0.0024</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1889,34 +2471,34 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M19">
         <v>0.01</v>
@@ -1927,34 +2509,34 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1965,54 +2547,60 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="14.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="26.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -2022,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2037,371 +2625,371 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F9" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add the Split feature in DamageDescriptionInPicture
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/外观检查.xlsx
+++ b/AutoRegularInspection/外观检查.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="136">
   <si>
     <t>序号</t>
   </si>
@@ -177,6 +177,27 @@
     <t>全桥栏杆多处表层油漆剥落、锈蚀</t>
   </si>
   <si>
+    <r>
+      <t>跨中栏杆表层油漆剥落、锈蚀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>$</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>全桥栏杆多处表层油漆剥落、锈蚀</t>
+    </r>
+  </si>
+  <si>
     <t>2743,2744</t>
   </si>
   <si>
@@ -443,12 +464,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -460,9 +481,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,22 +518,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -524,6 +544,14 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -568,7 +596,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -583,7 +611,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,28 +626,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -627,6 +638,132 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -636,73 +773,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -714,103 +803,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,16 +835,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -887,17 +898,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -912,61 +932,49 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -978,94 +986,97 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1394,12 +1405,13 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="36.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1731,11 +1743,11 @@
       <c r="E9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
@@ -1784,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1828,19 +1840,19 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -1866,19 +1878,19 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -1904,19 +1916,19 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -1942,19 +1954,19 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
@@ -1980,19 +1992,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I6" t="s">
         <v>19</v>
@@ -2018,19 +2030,19 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -2056,19 +2068,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I8" t="s">
         <v>19</v>
@@ -2094,19 +2106,19 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
@@ -2132,19 +2144,19 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
         <v>19</v>
@@ -2170,19 +2182,19 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I11" t="s">
         <v>19</v>
@@ -2208,19 +2220,19 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
@@ -2246,19 +2258,19 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I13" t="s">
         <v>19</v>
@@ -2270,7 +2282,7 @@
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M13">
         <v>0.0025</v>
@@ -2284,19 +2296,19 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I14" t="s">
         <v>19</v>
@@ -2308,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M14">
         <v>0.015</v>
@@ -2322,19 +2334,19 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I15" t="s">
         <v>19</v>
@@ -2346,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M15">
         <v>0.03</v>
@@ -2360,19 +2372,19 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" t="s">
         <v>19</v>
@@ -2384,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M16">
         <v>0.004</v>
@@ -2398,19 +2410,19 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I17" t="s">
         <v>19</v>
@@ -2422,7 +2434,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M17">
         <v>0.0025</v>
@@ -2436,19 +2448,19 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -2460,7 +2472,7 @@
         <v>1</v>
       </c>
       <c r="L18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M18">
         <v>0.0024</v>
@@ -2474,19 +2486,19 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I19" t="s">
         <v>19</v>
@@ -2498,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M19">
         <v>0.01</v>
@@ -2512,19 +2524,19 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I20" t="s">
         <v>19</v>
@@ -2550,19 +2562,19 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I21" t="s">
         <v>19</v>
@@ -2610,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2651,22 +2663,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I2" t="s">
         <v>19</v>
@@ -2689,22 +2701,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I3" t="s">
         <v>19</v>
@@ -2727,22 +2739,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -2765,22 +2777,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
@@ -2803,22 +2815,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I6" t="s">
         <v>19</v>
@@ -2841,22 +2853,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -2879,22 +2891,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I8" t="s">
         <v>19</v>
@@ -2917,22 +2929,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
@@ -2955,22 +2967,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I10" t="s">
         <v>19</v>

</xml_diff>